<commit_message>
update script and table
</commit_message>
<xml_diff>
--- a/Tables_v2.xlsx
+++ b/Tables_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgippet\Documents\Tmagnum_impacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE051DD-4A04-454E-A585-0BE70E69165A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54F7B38-E6F8-4232-AB05-8D08BECA49DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8325" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -1312,32 +1312,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1345,26 +1348,23 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1690,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="Q12" sqref="A4:Q12"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -1749,30 +1749,30 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="1:17" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="96" t="s">
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="91" t="s">
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="92" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="106.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="82"/>
-      <c r="B6" s="83"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="41" t="s">
         <v>23</v>
       </c>
@@ -1807,10 +1807,10 @@
       <c r="N6" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="90" t="s">
+      <c r="O6" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="92"/>
+      <c r="P6" s="93"/>
       <c r="Q6" s="46"/>
     </row>
     <row r="7" spans="1:17" s="2" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
@@ -1831,7 +1831,7 @@
       <c r="M7" s="79"/>
       <c r="N7" s="79"/>
       <c r="O7" s="22"/>
-      <c r="P7" s="93" t="s">
+      <c r="P7" s="83" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1853,7 +1853,7 @@
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
       <c r="O8" s="81"/>
-      <c r="P8" s="94" t="s">
+      <c r="P8" s="84" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1875,7 +1875,7 @@
       <c r="M9" s="19"/>
       <c r="N9" s="21"/>
       <c r="O9" s="37"/>
-      <c r="P9" s="94" t="s">
+      <c r="P9" s="84" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1897,7 +1897,7 @@
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
       <c r="O10" s="33"/>
-      <c r="P10" s="94" t="s">
+      <c r="P10" s="84" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1919,7 +1919,7 @@
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
       <c r="O11" s="38"/>
-      <c r="P11" s="95" t="s">
+      <c r="P11" s="85" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1946,7 +1946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174BE593-B72A-41F8-A77C-9DBD61C1AADF}">
   <dimension ref="B3:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G9" sqref="C9:G9"/>
     </sheetView>
   </sheetViews>
@@ -1960,20 +1960,20 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="87" t="s">
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="89"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="99"/>
     </row>
     <row r="5" spans="2:12" s="48" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="C5" s="49" t="s">

</xml_diff>